<commit_message>
Modified many names to nmrq_something and created setup.py and placeholder Readme.rst
</commit_message>
<xml_diff>
--- a/test_data/RawData_long.xlsx
+++ b/test_data/RawData_long.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20370"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20371"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\legregam\Documents\Projets\RMNQuant\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1826DC7-0506-449F-9BF3-D61E0EC2C3C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA9DB0A-C378-44DC-948F-B9F647C1222D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="29010" windowHeight="12510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -435,16 +435,16 @@
   <dimension ref="A1:Z31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1:V1048576"/>
+      <selection activeCell="Z2" sqref="Z2:Z31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,9 +524,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>7.8288000000000002</v>
@@ -602,12 +602,12 @@
         <v>21.247900000000001</v>
       </c>
       <c r="Z2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>7.9314999999999998</v>
@@ -683,12 +683,12 @@
         <v>20.425800000000002</v>
       </c>
       <c r="Z3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>7.9314999999999998</v>
@@ -764,12 +764,12 @@
         <v>19.7606</v>
       </c>
       <c r="Z4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>7.7068000000000003</v>
@@ -845,12 +845,12 @@
         <v>18.588699999999999</v>
       </c>
       <c r="Z5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>7.8402000000000003</v>
@@ -926,12 +926,12 @@
         <v>18.631499999999999</v>
       </c>
       <c r="Z6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>7.9269999999999996</v>
@@ -1007,12 +1007,12 @@
         <v>18.191100000000002</v>
       </c>
       <c r="Z7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>7.6744000000000003</v>
@@ -1088,12 +1088,12 @@
         <v>17.485900000000001</v>
       </c>
       <c r="Z8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>7.8231000000000002</v>
@@ -1169,12 +1169,12 @@
         <v>19.3506</v>
       </c>
       <c r="Z9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>7.9051</v>
@@ -1250,12 +1250,12 @@
         <v>19.5336</v>
       </c>
       <c r="Z10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>5.9606000000000003</v>
@@ -1331,12 +1331,12 @@
         <v>15.409099999999999</v>
       </c>
       <c r="Z11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>7.2990000000000004</v>
@@ -1412,12 +1412,12 @@
         <v>18.488</v>
       </c>
       <c r="Z12" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>7.5457999999999998</v>
@@ -1493,12 +1493,12 @@
         <v>19.244699999999998</v>
       </c>
       <c r="Z13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1">
         <v>7.2130000000000001</v>
@@ -1574,12 +1574,12 @@
         <v>18.759999999999998</v>
       </c>
       <c r="Z14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1">
         <v>7.2038000000000002</v>
@@ -1655,12 +1655,12 @@
         <v>18.941400000000002</v>
       </c>
       <c r="Z15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1">
         <v>6.5475000000000003</v>
@@ -1736,12 +1736,12 @@
         <v>17.3185</v>
       </c>
       <c r="Z16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
         <v>7.1696</v>
@@ -1817,12 +1817,12 @@
         <v>18.429899999999996</v>
       </c>
       <c r="Z17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
         <v>6.7156000000000002</v>
@@ -1898,12 +1898,12 @@
         <v>16.923699999999997</v>
       </c>
       <c r="Z18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1">
         <v>6.9246999999999996</v>
@@ -1979,12 +1979,12 @@
         <v>17.7866</v>
       </c>
       <c r="Z19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1">
         <v>7.4622000000000002</v>
@@ -2060,12 +2060,12 @@
         <v>17.843299999999999</v>
       </c>
       <c r="Z20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
         <v>7.1929999999999996</v>
@@ -2141,12 +2141,12 @@
         <v>15.663799999999998</v>
       </c>
       <c r="Z21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1">
         <v>6.7582000000000004</v>
@@ -2222,12 +2222,12 @@
         <v>15.490600000000001</v>
       </c>
       <c r="Z22" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
         <v>4.3556999999999997</v>
@@ -2303,12 +2303,12 @@
         <v>12.8401</v>
       </c>
       <c r="Z23" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1">
         <v>5.8106</v>
@@ -2384,12 +2384,12 @@
         <v>16.358899999999998</v>
       </c>
       <c r="Z24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>5.6971999999999996</v>
@@ -2465,12 +2465,12 @@
         <v>15.954599999999999</v>
       </c>
       <c r="Z25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1">
         <v>5.3484999999999996</v>
@@ -2546,12 +2546,12 @@
         <v>14.340299999999999</v>
       </c>
       <c r="Z26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1">
         <v>5.2914000000000003</v>
@@ -2627,12 +2627,12 @@
         <v>14.600200000000001</v>
       </c>
       <c r="Z27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1">
         <v>5.6795999999999998</v>
@@ -2708,12 +2708,12 @@
         <v>15.548999999999999</v>
       </c>
       <c r="Z28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1">
         <v>5.0007999999999999</v>
@@ -2789,12 +2789,12 @@
         <v>13.512499999999999</v>
       </c>
       <c r="Z29" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1">
         <v>4.8925000000000001</v>
@@ -2870,12 +2870,12 @@
         <v>12.774800000000003</v>
       </c>
       <c r="Z30" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1">
         <v>4.8239999999999998</v>
@@ -2951,7 +2951,7 @@
         <v>10.296700000000001</v>
       </c>
       <c r="Z31" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>